<commit_message>
fixing db_url replace for deployment
</commit_message>
<xml_diff>
--- a/tests/sample_data.xlsx
+++ b/tests/sample_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>title</t>
   </si>
@@ -27,15 +27,6 @@
     <t>title_short</t>
   </si>
   <si>
-    <t>navbar_logo</t>
-  </si>
-  <si>
-    <t>primary_colour</t>
-  </si>
-  <si>
-    <t>secondary_colour</t>
-  </si>
-  <si>
     <t>favicon_link</t>
   </si>
   <si>
@@ -49,9 +40,6 @@
   </si>
   <si>
     <t>google_analytics_key</t>
-  </si>
-  <si>
-    <t>G-tag script</t>
   </si>
   <si>
     <t>South African Candidates</t>
@@ -80,12 +68,57 @@
 "county_govenor": {"file": "CountyGovernor_Final.csv", "locator": ["county_name", "county_code"]}
 }</t>
   </si>
+  <si>
+    <t>gTag_script</t>
+  </si>
+  <si>
+    <t>organization_name</t>
+  </si>
+  <si>
+    <t>organization_link</t>
+  </si>
+  <si>
+    <t>logo_colour</t>
+  </si>
+  <si>
+    <t>footer_colour</t>
+  </si>
+  <si>
+    <t>body_foreground_colour</t>
+  </si>
+  <si>
+    <t>body_background_colour</t>
+  </si>
+  <si>
+    <t>find_candidates_button</t>
+  </si>
+  <si>
+    <t>candidate_names_colour</t>
+  </si>
+  <si>
+    <t>#FFC4AB</t>
+  </si>
+  <si>
+    <t>#1D3437</t>
+  </si>
+  <si>
+    <t>#30474A</t>
+  </si>
+  <si>
+    <t>#E5E5E5</t>
+  </si>
+  <si>
+    <t>#E07D54</t>
+  </si>
+  <si>
+    <t>#F2AA71</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +137,19 @@
       <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -149,6 +195,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -474,86 +532,99 @@
     <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:25" s="6" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="371.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-    </row>
-    <row r="2" spans="1:25" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="K2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>

</xml_diff>

<commit_message>
SA candidate iteration for build (#19)
* SA candidate iteration for build

* fixing db_url replace for deployment

* change color variables

---------

Co-authored-by: Ayanda Nene <ayandan@opencitieslab.org>
</commit_message>
<xml_diff>
--- a/tests/sample_data.xlsx
+++ b/tests/sample_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>title</t>
   </si>
@@ -27,15 +27,6 @@
     <t>title_short</t>
   </si>
   <si>
-    <t>navbar_logo</t>
-  </si>
-  <si>
-    <t>primary_colour</t>
-  </si>
-  <si>
-    <t>secondary_colour</t>
-  </si>
-  <si>
     <t>favicon_link</t>
   </si>
   <si>
@@ -49,9 +40,6 @@
   </si>
   <si>
     <t>google_analytics_key</t>
-  </si>
-  <si>
-    <t>G-tag script</t>
   </si>
   <si>
     <t>South African Candidates</t>
@@ -80,12 +68,57 @@
 "county_govenor": {"file": "CountyGovernor_Final.csv", "locator": ["county_name", "county_code"]}
 }</t>
   </si>
+  <si>
+    <t>gTag_script</t>
+  </si>
+  <si>
+    <t>organization_name</t>
+  </si>
+  <si>
+    <t>organization_link</t>
+  </si>
+  <si>
+    <t>logo_colour</t>
+  </si>
+  <si>
+    <t>footer_colour</t>
+  </si>
+  <si>
+    <t>body_foreground_colour</t>
+  </si>
+  <si>
+    <t>body_background_colour</t>
+  </si>
+  <si>
+    <t>find_candidates_button</t>
+  </si>
+  <si>
+    <t>candidate_names_colour</t>
+  </si>
+  <si>
+    <t>#FFC4AB</t>
+  </si>
+  <si>
+    <t>#1D3437</t>
+  </si>
+  <si>
+    <t>#30474A</t>
+  </si>
+  <si>
+    <t>#E5E5E5</t>
+  </si>
+  <si>
+    <t>#E07D54</t>
+  </si>
+  <si>
+    <t>#F2AA71</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +137,19 @@
       <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -149,6 +195,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -474,86 +532,99 @@
     <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:25" s="6" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="371.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-    </row>
-    <row r="2" spans="1:25" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="K2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>

</xml_diff>